<commit_message>
fixed the breaking code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -159,19 +159,19 @@
     <t>CustodianFilePath</t>
   </si>
   <si>
-    <t>C:\Users\decadev\Desktop\Pension_Reconciliation_Process_DDL\Data\Input\Custodian.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\decadev\Desktop\Pension_Reconciliation_Process_DDL\Data\Output</t>
-  </si>
-  <si>
     <t>OutputFilePath</t>
   </si>
   <si>
-    <t>C:\Users\decadev\Desktop\Pension_Reconciliation_Process_DDL\Data\Input\Employers\apple_inc.xlsx;C:\Users\decadev\Desktop\Pension_Reconciliation_Process_DDL\Data\Input\Employers\dell_inc.xlsx;C:\Users\decadev\Desktop\Pension_Reconciliation_Process_DDL\Data\Input\Employers\hp_inc.xlsx;C:\Users\decadev\Desktop\Pension_Reconciliation_Process_DDL\Data\Input\Employers\lenovo_inc.xlsx</t>
-  </si>
-  <si>
     <t>EmployerFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\Custodian.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
+  </si>
+  <si>
+    <t>Data\Input\Employers\apple_inc.xlsx;Data\Input\Employers\dell_inc.xlsx;Data\Input\Employers\hp_inc.xlsx;Data\Input\Employers\lenovo_inc.xlsx</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -635,15 +635,15 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -651,10 +651,10 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>